<commit_message>
Implementacion de vista para API Tics completa
</commit_message>
<xml_diff>
--- a/Back_end_python/db/tics.xlsx
+++ b/Back_end_python/db/tics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenin\Documents\GitHub\Proyecto_python\Back_end_python\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manrique\Desktop\Proyecto Python\Python_censo\Back_end_python\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9F5084-440E-48E9-953A-116198F3A17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60958760-51F1-42AE-B017-EAB9E26863B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="719" xr2:uid="{64AA4D7F-CF1A-4EC7-8C98-80366C114513}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="719" xr2:uid="{64AA4D7F-CF1A-4EC7-8C98-80366C114513}"/>
   </bookViews>
   <sheets>
     <sheet name="TICs" sheetId="26" r:id="rId1"/>
@@ -127,7 +127,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +180,14 @@
       <color theme="1"/>
       <name val="Museo Sans 100"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -264,7 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -297,15 +305,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -325,9 +334,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -365,7 +374,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -471,7 +480,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -613,7 +622,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -621,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF39B40-386A-4DC6-B645-684581DEDFBA}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -637,8 +646,8 @@
     <col min="9" max="9" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="63.75" customHeight="1" thickBot="1"/>
-    <row r="2" spans="1:8" ht="17.25" customHeight="1">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:8" ht="49.5">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -678,7 +687,7 @@
         <v>49158</v>
       </c>
       <c r="E3" s="7">
-        <v>230144</v>
+        <v>49158</v>
       </c>
       <c r="F3" s="7">
         <v>36915</v>
@@ -1054,8 +1063,12 @@
         <v>5634803</v>
       </c>
     </row>
+    <row r="27" spans="1:8">
+      <c r="F27" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1070,28 +1083,28 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="19.5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" thickBot="1">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" ht="66">
       <c r="A3" s="6" t="s">
@@ -1510,16 +1523,16 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9">
@@ -1543,28 +1556,28 @@
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="19.5">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
     </row>
     <row r="24" spans="1:9" ht="20.25" thickBot="1">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="1:9" ht="66">
       <c r="A25" s="6" t="s">
@@ -1983,16 +1996,16 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1"/>
@@ -2016,38 +2029,18 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A41:H41"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A23:H23"/>
     <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A41:H41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="27160ef2-b1a0-4e0b-a979-9938934b2ceb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="313f4996-b919-4f00-b21c-15f2583e5308" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009DCC8FD18B82734DA6D04F28797DC4A6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d6bdc30562d183d288a9000ae6c88d0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="27160ef2-b1a0-4e0b-a979-9938934b2ceb" xmlns:ns3="313f4996-b919-4f00-b21c-15f2583e5308" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb1f178905c4cbe79baa28c8245f5f7a" ns2:_="" ns3:_="">
     <xsd:import namespace="27160ef2-b1a0-4e0b-a979-9938934b2ceb"/>
@@ -2276,26 +2269,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55415A4B-DEE3-487D-9856-B67DBCF2CBCC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="27160ef2-b1a0-4e0b-a979-9938934b2ceb"/>
-    <ds:schemaRef ds:uri="313f4996-b919-4f00-b21c-15f2583e5308"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C923171F-D5BD-4E16-AC37-684330A08399}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="27160ef2-b1a0-4e0b-a979-9938934b2ceb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="313f4996-b919-4f00-b21c-15f2583e5308" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6D4EC8A-7851-4DAA-A5DD-796CDC950495}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2312,4 +2306,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C923171F-D5BD-4E16-AC37-684330A08399}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55415A4B-DEE3-487D-9856-B67DBCF2CBCC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="27160ef2-b1a0-4e0b-a979-9938934b2ceb"/>
+    <ds:schemaRef ds:uri="313f4996-b919-4f00-b21c-15f2583e5308"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>